<commit_message>
aanpasssingen in alle diagrammen aangegeven
</commit_message>
<xml_diff>
--- a/uml/IMKL2.x/IMKL-UML-changelog.xlsx
+++ b/uml/IMKL2.x/IMKL-UML-changelog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjanssen\Documents\GitHub\imkl2015-dev\uml\IMKL2.x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5C81F2-9595-420B-B59A-956E99721E7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F189FFA-84E6-4EF5-B9B5-AF92E1EC1DC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="0" windowWidth="10890" windowHeight="13935" xr2:uid="{894B1FF5-8DFC-4651-A7C4-67B2EE5B0E46}"/>
+    <workbookView xWindow="-17580" yWindow="-6285" windowWidth="15210" windowHeight="13935" xr2:uid="{894B1FF5-8DFC-4651-A7C4-67B2EE5B0E46}"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="106">
   <si>
     <t>Datum</t>
   </si>
@@ -355,6 +355,12 @@
   </si>
   <si>
     <t>CONTROLEER DESCRIPTION</t>
+  </si>
+  <si>
+    <t>ContainerLeidingelement-VRAAG:ook max 1 utiliteitsnet???</t>
+  </si>
+  <si>
+    <t>VRAAG: moet dat niet ook in XSD?</t>
   </si>
 </sst>
 </file>
@@ -416,7 +422,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -426,6 +432,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -444,7 +456,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -487,7 +499,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -810,7 +825,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="B47" sqref="B44:B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1360,7 +1375,9 @@
       <c r="B24" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="7"/>
+      <c r="C24" s="16" t="s">
+        <v>105</v>
+      </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7" t="s">
@@ -1759,7 +1776,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="16" t="s">
         <v>98</v>
       </c>
       <c r="C44" s="7"/>
@@ -1774,7 +1791,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="7"/>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="17" t="s">
         <v>100</v>
       </c>
       <c r="C45" s="7"/>
@@ -1789,7 +1806,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="17" t="s">
         <v>102</v>
       </c>
       <c r="C46" s="7"/>
@@ -1802,9 +1819,11 @@
       <c r="H46" s="9"/>
       <c r="I46" s="8"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
+      <c r="B47" s="16" t="s">
+        <v>104</v>
+      </c>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
@@ -3447,15 +3466,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003ADD3040E3157B4E913BCA65F34844D7" ma:contentTypeVersion="10" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c1765059aa1475931adc12138fdcfd8c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aafb19fa-82be-411d-a6df-c75e9235a4ea" xmlns:ns3="3dfebdfe-2b22-40ba-8672-9fbc9b4066c4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="42d79c55539af1f9f274032ce6041302" ns2:_="" ns3:_="">
     <xsd:import namespace="aafb19fa-82be-411d-a6df-c75e9235a4ea"/>
@@ -3658,6 +3668,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB1489CD-B12A-4704-A7E2-006D773FFFBF}">
   <ds:schemaRefs>
@@ -3668,14 +3687,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7893A73B-81F0-482A-B793-D93E5F8DCA71}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0C9FDDB-2830-4DD6-A847-D844746B12F8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3692,4 +3703,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7893A73B-81F0-482A-B793-D93E5F8DCA71}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
alle diagrammen met wijzigingskaders
</commit_message>
<xml_diff>
--- a/uml/IMKL2.x/IMKL-UML-changelog.xlsx
+++ b/uml/IMKL2.x/IMKL-UML-changelog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjanssen\Documents\GitHub\imkl2015-dev\uml\IMKL2.x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F189FFA-84E6-4EF5-B9B5-AF92E1EC1DC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1457B5D2-6D88-4BE8-B8AA-86671D07517F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17580" yWindow="-6285" windowWidth="15210" windowHeight="13935" xr2:uid="{894B1FF5-8DFC-4651-A7C4-67B2EE5B0E46}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{894B1FF5-8DFC-4651-A7C4-67B2EE5B0E46}"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="114">
   <si>
     <t>Datum</t>
   </si>
@@ -342,32 +342,90 @@
     <t>Graafpolygoon</t>
   </si>
   <si>
-    <t>CONTROLEER REFERENTIE AAN WION</t>
-  </si>
-  <si>
     <t>Informatiepolygoon:</t>
   </si>
   <si>
-    <t>CONTROLEEER GEEN DEFINITIE</t>
-  </si>
-  <si>
     <t>Leidingelement:</t>
   </si>
   <si>
-    <t>CONTROLEER DESCRIPTION</t>
-  </si>
-  <si>
-    <t>ContainerLeidingelement-VRAAG:ook max 1 utiliteitsnet???</t>
-  </si>
-  <si>
-    <t>VRAAG: moet dat niet ook in XSD?</t>
+    <t>ContainerLeidingelement</t>
+  </si>
+  <si>
+    <t>Toren</t>
+  </si>
+  <si>
+    <t>Mast</t>
+  </si>
+  <si>
+    <t>Mangat</t>
+  </si>
+  <si>
+    <t>Kast</t>
+  </si>
+  <si>
+    <t>TechnischGebouw</t>
+  </si>
+  <si>
+    <t>Duct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source was: Artikel1 WION; wordt Artikel 1 WIBON
+</t>
+  </si>
+  <si>
+    <t>Orientatiepolygoon</t>
+  </si>
+  <si>
+    <t>hoeft niet in XSD</t>
+  </si>
+  <si>
+    <t>was: geen definitie
+wordt: 
+definition: Een informatiepolygoon is de weergave door een grondroerder van het gebied, waarvoor gebiedsinformatie wordt gevraagd.
+Description: De gebiedsinformatie die zich bevindt tussen een informatiepolygoon en de graafpolygoon is puur ter informatie en ondersteuning van de werkzaamheden van de grondroerder.</t>
+  </si>
+  <si>
+    <t>was: Gebied dat een persoon of organisatie tekent om daar informatie over kabels en leidingen van te ontvangen.
+wordt: Een oriëntatiepolygoon is de weergave door een opdrachtgever, grondroerder, aanbieder of bestuursorgaan van een aangesloten gebied, ten aanzien waarvan deze om gebiedsinformatie verzoekt met het oog op respectievelijk het voorbereiden van graafwerkzaamheden, het voorbereiden van een verzoek tot medegebruik of coördinatie, of ten behoeve van de hem opgedragen taak.
+ --Source--Artikel 1 en Artikel 7 WIBON</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Was: Description: Bijvoorbeeld objecten zoals een schakelkast, verdeelkast, kranen, afsluiters, versterkers, kabelmof, rioolput, (druk)rioolgemaal, kathodische bescherming, boorput, etc. 
+In de WION hebben “elementen” betrekking op ondergrondse delen van het net, terwijl “markeringen” betrekking hebben op bovengrondse delen. Een leidingelement in het IMKL kan zowel betrekking hebben op ondergrondse als op bovengrondse delen van het net.
+Optioneel is er via het associatie-attribuut extraGeometrie een buitenbegrenzing of contour van het object op te nemen. De netbeheerder bepaalt zelf wanneer dat functioneel is.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wordt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Description: Bijvoorbeeld objecten zoals een schakelkast, verdeelkast, kranen, afsluiters, versterkers, kabelmof, rioolput, (druk)rioolgemaal, kathodische bescherming, boorput, etc. 
+Een leidingelement kan zowel betrekking hebben op ondergrondse als op bovengrondse delen van het net.
+Optioneel is er via het associatie-attribuut extraGeometrie een buitenbegrenzing of contour van het object op te nemen. De netbeheerder bepaalt zelf wanneer dat functioneel is.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -421,6 +479,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -437,7 +503,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,7 +522,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -499,11 +565,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -824,8 +893,8 @@
   <dimension ref="A1:M180"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B47" sqref="B44:B47"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1375,15 +1444,15 @@
       <c r="B24" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="16" t="s">
-        <v>105</v>
-      </c>
+      <c r="C24" s="18"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="7"/>
+      <c r="G24" s="7" t="s">
+        <v>110</v>
+      </c>
       <c r="H24" s="9"/>
       <c r="I24" s="7"/>
     </row>
@@ -1774,8 +1843,10 @@
       <c r="H43" s="9"/>
       <c r="I43" s="8"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="7"/>
+    <row r="44" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A44" s="7">
+        <v>43990</v>
+      </c>
       <c r="B44" s="16" t="s">
         <v>98</v>
       </c>
@@ -1783,139 +1854,243 @@
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
       <c r="F44" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="G44" s="7"/>
+        <v>108</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="H44" s="9"/>
       <c r="I44" s="8"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="7"/>
+    <row r="45" spans="1:9" ht="152.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="7">
+        <v>43990</v>
+      </c>
       <c r="B45" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
       <c r="F45" s="7" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="G45" s="7"/>
       <c r="H45" s="9"/>
       <c r="I45" s="8"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="7"/>
+    <row r="46" spans="1:9" ht="290.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="7">
+        <v>43990</v>
+      </c>
       <c r="B46" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="G46" s="7"/>
       <c r="H46" s="9"/>
       <c r="I46" s="8"/>
     </row>
-    <row r="47" spans="1:9" ht="24" x14ac:dyDescent="0.2">
-      <c r="A47" s="7"/>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="7">
+        <v>43990</v>
+      </c>
       <c r="B47" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G47" s="7"/>
+      <c r="H47" s="9">
+        <v>269</v>
+      </c>
+      <c r="I47" s="8"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="7">
+        <v>43990</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G48" s="7"/>
+      <c r="H48" s="9">
+        <v>269</v>
+      </c>
+      <c r="I48" s="8"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="7">
+        <v>43990</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G49" s="7"/>
+      <c r="H49" s="9">
+        <v>269</v>
+      </c>
+      <c r="I49" s="8"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" s="7">
+        <v>43990</v>
+      </c>
+      <c r="B50" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="8"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="8"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="8"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
+      <c r="C50" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
+      <c r="E50" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="G50" s="7"/>
-      <c r="H50" s="9"/>
+      <c r="H50" s="9">
+        <v>269</v>
+      </c>
       <c r="I50" s="8"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
+      <c r="A51" s="7">
+        <v>43990</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
+      <c r="E51" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="G51" s="7"/>
-      <c r="H51" s="9"/>
+      <c r="H51" s="9">
+        <v>269</v>
+      </c>
       <c r="I51" s="8"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
+      <c r="A52" s="7">
+        <v>43990</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
+      <c r="E52" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="G52" s="7"/>
-      <c r="H52" s="9"/>
+      <c r="H52" s="9">
+        <v>269</v>
+      </c>
       <c r="I52" s="8"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
+      <c r="A53" s="7">
+        <v>43990</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
+      <c r="E53" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="G53" s="7"/>
-      <c r="H53" s="9"/>
+      <c r="H53" s="9">
+        <v>269</v>
+      </c>
       <c r="I53" s="8"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
+      <c r="A54" s="7">
+        <v>43990</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
+      <c r="E54" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="G54" s="7"/>
-      <c r="H54" s="9"/>
+      <c r="H54" s="9">
+        <v>269</v>
+      </c>
       <c r="I54" s="8"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="144" x14ac:dyDescent="0.2">
       <c r="A55" s="7"/>
-      <c r="B55" s="7"/>
+      <c r="B55" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
+      <c r="F55" s="16" t="s">
+        <v>112</v>
+      </c>
       <c r="G55" s="7"/>
       <c r="H55" s="9"/>
       <c r="I55" s="8"/>
@@ -3466,6 +3641,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003ADD3040E3157B4E913BCA65F34844D7" ma:contentTypeVersion="10" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c1765059aa1475931adc12138fdcfd8c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aafb19fa-82be-411d-a6df-c75e9235a4ea" xmlns:ns3="3dfebdfe-2b22-40ba-8672-9fbc9b4066c4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="42d79c55539af1f9f274032ce6041302" ns2:_="" ns3:_="">
     <xsd:import namespace="aafb19fa-82be-411d-a6df-c75e9235a4ea"/>
@@ -3668,15 +3852,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB1489CD-B12A-4704-A7E2-006D773FFFBF}">
   <ds:schemaRefs>
@@ -3687,6 +3862,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7893A73B-81F0-482A-B793-D93E5F8DCA71}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0C9FDDB-2830-4DD6-A847-D844746B12F8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3703,12 +3886,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7893A73B-81F0-482A-B793-D93E5F8DCA71}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>